<commit_message>
Manage news test cases
</commit_message>
<xml_diff>
--- a/GroceryApplication/src/test/resources/TestData.xlsx
+++ b/GroceryApplication/src/test/resources/TestData.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silpa\git\GroceryApplicationProject\GroceryApplication\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18456" windowHeight="5628" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18456" windowHeight="5628"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="HomePage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -423,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,6 +487,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -492,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>